<commit_message>
KIBON-120: Gesuch-Stichtag statistic translated
</commit_message>
<xml_diff>
--- a/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
+++ b/ebegu-server/src/main/resources/reporting/GesuchStichtag.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="7" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\Client\A$\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E69296D4-C4F1-4FB5-93C3-EBD57A7D2911}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="14010" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Report" sheetId="1" r:id="rId1"/>
@@ -17,8 +23,8 @@
   <pivotCaches>
     <pivotCache cacheId="5" r:id="rId3"/>
   </pivotCaches>
-  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -26,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>Institution</t>
   </si>
@@ -37,18 +43,6 @@
     <t>Periode</t>
   </si>
   <si>
-    <t>NichtFreigegeben</t>
-  </si>
-  <si>
-    <t>Mahnungen</t>
-  </si>
-  <si>
-    <t>Beschwerde</t>
-  </si>
-  <si>
-    <t>BGNummer</t>
-  </si>
-  <si>
     <t>{bgNummer}</t>
   </si>
   <si>
@@ -85,20 +79,41 @@
     <t>Values</t>
   </si>
   <si>
-    <t>GesuchLaufNr</t>
-  </si>
-  <si>
     <t>{gesuchLaufNr}</t>
   </si>
   <si>
     <t>(Alle)</t>
+  </si>
+  <si>
+    <t>{gesuchLaufNrTitle}</t>
+  </si>
+  <si>
+    <t>{nichtFreigegebenTitle}</t>
+  </si>
+  <si>
+    <t>{bgNummerTitle}</t>
+  </si>
+  <si>
+    <t>{institutionTitle}</t>
+  </si>
+  <si>
+    <t>{angebotTitle}</t>
+  </si>
+  <si>
+    <t>{periodeTitle}</t>
+  </si>
+  <si>
+    <t>{mahnungenTitle}</t>
+  </si>
+  <si>
+    <t>{beschwerdeTitle}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,272 +183,7 @@
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="56">
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <left style="thin">
-          <color theme="1"/>
-        </left>
-        <right style="thin">
-          <color theme="1"/>
-        </right>
-        <top style="thin">
-          <color theme="1"/>
-        </top>
-        <bottom style="thin">
-          <color theme="1"/>
-        </bottom>
-        <vertical style="thin">
-          <color theme="1"/>
-        </vertical>
-        <horizontal style="thin">
-          <color theme="1"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-    </dxf>
+  <dxfs count="28">
     <dxf>
       <font>
         <b val="0"/>
@@ -713,7 +463,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshOnLoad="1" refreshedBy="Franziska Herger" refreshedDate="42992.666940277777" createdVersion="6" refreshedVersion="3" minRefreshableVersion="3" recordCount="1">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" r:id="rId1" refreshOnLoad="1" refreshedBy="Bernabeu Imanol" refreshedDate="43482.409256134262" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="1" xr:uid="{00000000-000A-0000-FFFF-FFFF05000000}">
   <cacheSource type="worksheet">
     <worksheetSource name="GesuchStichtagPivottableData"/>
   </cacheSource>
@@ -758,7 +508,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="1">
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" count="1">
   <r>
     <s v="{bgNummer}"/>
     <x v="0"/>
@@ -773,7 +523,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="3" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable4" cacheId="5" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" compact="0" outline="1" outlineData="1" compactData="0" multipleFieldFilters="0">
   <location ref="B4:F7" firstHeaderRow="1" firstDataRow="2" firstDataCol="2" rowPageCount="1" colPageCount="1"/>
   <pivotFields count="8">
     <pivotField compact="0" showAll="0" defaultSubtotal="0"/>
@@ -832,26 +582,26 @@
     <dataField name="Offene Beschwerden" fld="7" baseField="0" baseItem="0"/>
   </dataFields>
   <formats count="28">
-    <format dxfId="55">
+    <format dxfId="27">
       <pivotArea type="all" dataOnly="0" outline="0" fieldPosition="0"/>
     </format>
-    <format dxfId="54">
+    <format dxfId="26">
       <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
     </format>
-    <format dxfId="53">
+    <format dxfId="25">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="52">
+    <format dxfId="24">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="51">
+    <format dxfId="23">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="50">
+    <format dxfId="22">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -859,7 +609,7 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="49">
+    <format dxfId="21">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -870,13 +620,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="48">
+    <format dxfId="20">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="47">
+    <format dxfId="19">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="46">
+    <format dxfId="18">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -887,13 +637,13 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="45">
+    <format dxfId="17">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="44">
+    <format dxfId="16">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="43">
+    <format dxfId="15">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="4294967294" count="3">
@@ -904,23 +654,23 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="42">
+    <format dxfId="14">
       <pivotArea field="3" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisPage" fieldPosition="0"/>
     </format>
-    <format dxfId="41">
+    <format dxfId="13">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="40">
+    <format dxfId="12">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="39">
+    <format dxfId="11">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="38">
+    <format dxfId="10">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -928,20 +678,20 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="37">
+    <format dxfId="9">
       <pivotArea field="1" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="0"/>
     </format>
-    <format dxfId="36">
+    <format dxfId="8">
       <pivotArea field="2" type="button" dataOnly="0" labelOnly="1" outline="0" axis="axisRow" fieldPosition="1"/>
     </format>
-    <format dxfId="35">
+    <format dxfId="7">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="34">
+    <format dxfId="6">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -949,14 +699,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="33">
+    <format dxfId="5">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="32">
+    <format dxfId="4">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -964,14 +714,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="31">
+    <format dxfId="3">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="30">
+    <format dxfId="2">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -979,14 +729,14 @@
         </references>
       </pivotArea>
     </format>
-    <format dxfId="29">
+    <format dxfId="1">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="1">
           <reference field="1" count="0"/>
         </references>
       </pivotArea>
     </format>
-    <format dxfId="28">
+    <format dxfId="0">
       <pivotArea dataOnly="0" labelOnly="1" outline="0" fieldPosition="0">
         <references count="2">
           <reference field="1" count="0" selected="0"/>
@@ -1293,19 +1043,19 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="21.42578125" customWidth="1"/>
     <col min="3" max="3" width="16.5703125" bestFit="1" customWidth="1"/>
@@ -1336,24 +1086,24 @@
     <col min="28" max="28" width="35.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:6">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="4" spans="2:6">
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="6" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="2:6">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
         <v>0</v>
       </c>
@@ -1361,28 +1111,28 @@
         <v>1</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:6">
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B6" s="5" t="s">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="C6" s="1"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
     </row>
-    <row r="7" spans="2:6">
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B7" s="5"/>
       <c r="C7" s="5" t="s">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="D7" s="2">
         <v>0</v>
@@ -1400,14 +1150,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" customWidth="1"/>
     <col min="2" max="2" width="29.28515625" customWidth="1"/>
@@ -1419,59 +1169,59 @@
     <col min="8" max="8" width="16.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B1" t="s">
+        <v>20</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>22</v>
+      </c>
+      <c r="E1" t="s">
+        <v>17</v>
+      </c>
+      <c r="F1" t="s">
+        <v>18</v>
+      </c>
+      <c r="G1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="B1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" t="s">
-        <v>19</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
-      <c r="A2" t="s">
+      <c r="E2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="G2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="H2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="I2" t="s">
         <v>10</v>
-      </c>
-      <c r="E2" t="s">
-        <v>20</v>
-      </c>
-      <c r="F2" t="s">
-        <v>11</v>
-      </c>
-      <c r="G2" t="s">
-        <v>12</v>
-      </c>
-      <c r="H2" t="s">
-        <v>13</v>
-      </c>
-      <c r="I2" t="s">
-        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>